<commit_message>
checking in the new tests and the changes made in some files .
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Check_EvidenceMagnifyingGlass_VerticallyAligned.xlsx
+++ b/src/main/resources/testdata/Check_EvidenceMagnifyingGlass_VerticallyAligned.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2130" yWindow="2130" windowWidth="12945" windowHeight="3990"/>
+    <workbookView xWindow="2130" yWindow="2190" windowWidth="12945" windowHeight="3930"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Data#</t>
   </si>
@@ -32,9 +31,6 @@
   </si>
   <si>
     <t>selectType</t>
-  </si>
-  <si>
-    <t>Elkomy,Mohamed</t>
   </si>
   <si>
     <t>RNAi</t>
@@ -104,6 +100,15 @@
   </si>
   <si>
     <t>evidence</t>
+  </si>
+  <si>
+    <t>Nisha, Pillai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akhavan Rezayat A, Katebi M. </t>
+  </si>
+  <si>
+    <t>basal root thickness [en;XX;1]</t>
   </si>
 </sst>
 </file>
@@ -456,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,15 +474,15 @@
     <col min="3" max="3" width="23.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="22.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="34.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="21.42578125" style="1" customWidth="1"/>
     <col min="8" max="9" width="22.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="24.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="29.7109375" style="1" customWidth="1"/>
     <col min="11" max="11" width="21" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,25 +496,25 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -517,28 +522,51 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>